<commit_message>
IISIM Linux 3.0.0-alpha.7: DialogEULA, Debugging - Finished implementation of DialogEULA... UI & elements - Debugged GTK window parenting and positioning
</commit_message>
<xml_diff>
--- a/II Library, C#/Localization Strings.xlsx
+++ b/II Library, C#/Localization Strings.xlsx
@@ -14349,7 +14349,7 @@
     <t>EULA:AgreeToTerms</t>
   </si>
   <si>
-    <t xml:space="preserve">By choosing to continue, you accept to the terms of use at located at</t>
+    <t xml:space="preserve">By choosing to continue, you accept to the terms of use:</t>
   </si>
   <si>
     <t xml:space="preserve">ከቀጠሉ በአጠቃቀም ውል ተስማምተዋል</t>
@@ -15440,7 +15440,6 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -15499,9 +15498,6 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -15510,6 +15506,9 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -19636,7 +19635,7 @@
       </c>
     </row>
     <row r="80" s="1" customFormat="1">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="1" t="s">
         <v>1100</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -19686,10 +19685,10 @@
       </c>
     </row>
     <row r="81" s="1" customFormat="1">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="1" t="s">
         <v>1116</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -20787,10 +20786,10 @@
       </c>
     </row>
     <row r="104" s="1" customFormat="1">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="5" t="s">
         <v>1457</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="5" t="s">
         <v>1101</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -25383,10 +25382,10 @@
       </c>
     </row>
     <row r="202" s="1" customFormat="1">
-      <c r="A202" s="7" t="s">
+      <c r="A202" s="6" t="s">
         <v>2814</v>
       </c>
-      <c r="B202" s="7" t="s">
+      <c r="B202" s="6" t="s">
         <v>2815</v>
       </c>
       <c r="C202" s="1" t="s">
@@ -25433,10 +25432,10 @@
       </c>
     </row>
     <row r="203" s="1" customFormat="1">
-      <c r="A203" s="7" t="s">
+      <c r="A203" s="6" t="s">
         <v>2829</v>
       </c>
-      <c r="B203" s="7" t="s">
+      <c r="B203" s="6" t="s">
         <v>2830</v>
       </c>
       <c r="C203" s="1" t="s">
@@ -25483,10 +25482,10 @@
       </c>
     </row>
     <row r="204" s="1" customFormat="1">
-      <c r="A204" s="7" t="s">
+      <c r="A204" s="6" t="s">
         <v>2836</v>
       </c>
-      <c r="B204" s="7" t="s">
+      <c r="B204" s="6" t="s">
         <v>2837</v>
       </c>
       <c r="C204" s="1" t="s">
@@ -25533,10 +25532,10 @@
       </c>
     </row>
     <row r="205" s="1" customFormat="1">
-      <c r="A205" s="7" t="s">
+      <c r="A205" s="6" t="s">
         <v>2844</v>
       </c>
-      <c r="B205" s="7" t="s">
+      <c r="B205" s="6" t="s">
         <v>2845</v>
       </c>
       <c r="C205" s="1" t="s">
@@ -25583,10 +25582,10 @@
       </c>
     </row>
     <row r="206" s="1" customFormat="1">
-      <c r="A206" s="7" t="s">
+      <c r="A206" s="6" t="s">
         <v>2860</v>
       </c>
-      <c r="B206" s="7" t="s">
+      <c r="B206" s="6" t="s">
         <v>2861</v>
       </c>
       <c r="C206" s="1" t="s">
@@ -25633,10 +25632,10 @@
       </c>
     </row>
     <row r="207" s="1" customFormat="1">
-      <c r="A207" s="7" t="s">
+      <c r="A207" s="6" t="s">
         <v>2862</v>
       </c>
-      <c r="B207" s="7" t="s">
+      <c r="B207" s="6" t="s">
         <v>2863</v>
       </c>
       <c r="C207" s="1" t="s">
@@ -25683,10 +25682,10 @@
       </c>
     </row>
     <row r="208" s="1" customFormat="1">
-      <c r="A208" s="7" t="s">
+      <c r="A208" s="6" t="s">
         <v>2878</v>
       </c>
-      <c r="B208" s="7" t="s">
+      <c r="B208" s="6" t="s">
         <v>2879</v>
       </c>
       <c r="C208" s="1" t="s">
@@ -25733,10 +25732,10 @@
       </c>
     </row>
     <row r="209" s="1" customFormat="1">
-      <c r="A209" s="7" t="s">
+      <c r="A209" s="6" t="s">
         <v>2890</v>
       </c>
-      <c r="B209" s="7" t="s">
+      <c r="B209" s="6" t="s">
         <v>2799</v>
       </c>
       <c r="C209" s="1" t="s">
@@ -25783,10 +25782,10 @@
       </c>
     </row>
     <row r="210" s="1" customFormat="1">
-      <c r="A210" s="7" t="s">
+      <c r="A210" s="6" t="s">
         <v>2893</v>
       </c>
-      <c r="B210" s="7" t="s">
+      <c r="B210" s="6" t="s">
         <v>2894</v>
       </c>
       <c r="C210" s="1" t="s">
@@ -25833,10 +25832,10 @@
       </c>
     </row>
     <row r="211" s="1" customFormat="1">
-      <c r="A211" s="7" t="s">
+      <c r="A211" s="6" t="s">
         <v>2907</v>
       </c>
-      <c r="B211" s="7" t="s">
+      <c r="B211" s="6" t="s">
         <v>2908</v>
       </c>
       <c r="C211" s="1" t="s">
@@ -25883,10 +25882,10 @@
       </c>
     </row>
     <row r="212" s="1" customFormat="1">
-      <c r="A212" s="7" t="s">
+      <c r="A212" s="6" t="s">
         <v>2923</v>
       </c>
-      <c r="B212" s="7" t="s">
+      <c r="B212" s="6" t="s">
         <v>2924</v>
       </c>
       <c r="C212" s="1" t="s">
@@ -25933,10 +25932,10 @@
       </c>
     </row>
     <row r="213" s="1" customFormat="1">
-      <c r="A213" s="7" t="s">
+      <c r="A213" s="6" t="s">
         <v>2939</v>
       </c>
-      <c r="B213" s="7" t="s">
+      <c r="B213" s="6" t="s">
         <v>2519</v>
       </c>
       <c r="C213" s="1" t="s">
@@ -25966,7 +25965,7 @@
       <c r="K213" s="1" t="s">
         <v>2940</v>
       </c>
-      <c r="L213" s="8" t="s">
+      <c r="L213" s="7" t="s">
         <v>2941</v>
       </c>
       <c r="M213" s="1" t="s">
@@ -25983,10 +25982,10 @@
       </c>
     </row>
     <row r="214" s="1" customFormat="1">
-      <c r="A214" s="7" t="s">
+      <c r="A214" s="6" t="s">
         <v>2944</v>
       </c>
-      <c r="B214" s="7" t="s">
+      <c r="B214" s="6" t="s">
         <v>2945</v>
       </c>
       <c r="C214" s="1" t="s">
@@ -26033,10 +26032,10 @@
       </c>
     </row>
     <row r="215" s="1" customFormat="1">
-      <c r="A215" s="7" t="s">
+      <c r="A215" s="6" t="s">
         <v>2960</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B215" s="6" t="s">
         <v>2961</v>
       </c>
       <c r="C215" s="1" t="s">
@@ -26080,10 +26079,10 @@
       </c>
     </row>
     <row r="216" s="1" customFormat="1">
-      <c r="A216" s="7" t="s">
+      <c r="A216" s="6" t="s">
         <v>2975</v>
       </c>
-      <c r="B216" s="7" t="s">
+      <c r="B216" s="6" t="s">
         <v>2976</v>
       </c>
       <c r="C216" s="1" t="s">
@@ -26127,10 +26126,10 @@
       </c>
     </row>
     <row r="217" s="1" customFormat="1">
-      <c r="A217" s="7" t="s">
+      <c r="A217" s="6" t="s">
         <v>2984</v>
       </c>
-      <c r="B217" s="7" t="s">
+      <c r="B217" s="6" t="s">
         <v>2985</v>
       </c>
       <c r="C217" s="1" t="s">
@@ -26177,10 +26176,10 @@
       </c>
     </row>
     <row r="218" s="1" customFormat="1">
-      <c r="A218" s="7" t="s">
+      <c r="A218" s="6" t="s">
         <v>2999</v>
       </c>
-      <c r="B218" s="7" t="s">
+      <c r="B218" s="6" t="s">
         <v>3000</v>
       </c>
       <c r="C218" s="1" t="s">
@@ -26224,10 +26223,10 @@
       </c>
     </row>
     <row r="219" s="1" customFormat="1">
-      <c r="A219" s="7" t="s">
+      <c r="A219" s="6" t="s">
         <v>3001</v>
       </c>
-      <c r="B219" s="7" t="s">
+      <c r="B219" s="6" t="s">
         <v>3002</v>
       </c>
       <c r="C219" s="1" t="s">
@@ -26271,14 +26270,14 @@
       </c>
     </row>
     <row r="220" s="1" customFormat="1">
-      <c r="A220" s="7"/>
-      <c r="B220" s="7"/>
+      <c r="A220" s="6"/>
+      <c r="B220" s="6"/>
     </row>
     <row r="221" s="1" customFormat="1">
-      <c r="A221" s="7" t="s">
+      <c r="A221" s="6" t="s">
         <v>3003</v>
       </c>
-      <c r="B221" s="7" t="s">
+      <c r="B221" s="6" t="s">
         <v>3004</v>
       </c>
       <c r="C221" s="1" t="s">
@@ -26325,10 +26324,10 @@
       </c>
     </row>
     <row r="222" s="1" customFormat="1">
-      <c r="A222" s="7" t="s">
+      <c r="A222" s="6" t="s">
         <v>3005</v>
       </c>
-      <c r="B222" s="7" t="s">
+      <c r="B222" s="6" t="s">
         <v>3006</v>
       </c>
       <c r="C222" s="1" t="s">
@@ -26375,10 +26374,10 @@
       </c>
     </row>
     <row r="223" s="1" customFormat="1">
-      <c r="A223" s="7" t="s">
+      <c r="A223" s="6" t="s">
         <v>3021</v>
       </c>
-      <c r="B223" s="7" t="s">
+      <c r="B223" s="6" t="s">
         <v>3022</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -26425,10 +26424,10 @@
       </c>
     </row>
     <row r="224" s="1" customFormat="1">
-      <c r="A224" s="7" t="s">
+      <c r="A224" s="6" t="s">
         <v>3037</v>
       </c>
-      <c r="B224" s="7" t="s">
+      <c r="B224" s="6" t="s">
         <v>3038</v>
       </c>
       <c r="C224" s="1" t="s">
@@ -26475,10 +26474,10 @@
       </c>
     </row>
     <row r="225" s="1" customFormat="1">
-      <c r="A225" s="7" t="s">
+      <c r="A225" s="6" t="s">
         <v>3053</v>
       </c>
-      <c r="B225" s="7" t="s">
+      <c r="B225" s="6" t="s">
         <v>3054</v>
       </c>
       <c r="C225" s="1" t="s">
@@ -26525,10 +26524,10 @@
       </c>
     </row>
     <row r="226" s="1" customFormat="1">
-      <c r="A226" s="7" t="s">
+      <c r="A226" s="6" t="s">
         <v>3069</v>
       </c>
-      <c r="B226" s="7" t="s">
+      <c r="B226" s="6" t="s">
         <v>3070</v>
       </c>
       <c r="C226" s="1" t="s">
@@ -26928,49 +26927,49 @@
       <c r="A234" s="1" t="s">
         <v>3191</v>
       </c>
-      <c r="B234" s="9" t="s">
+      <c r="B234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="C234" s="9" t="s">
+      <c r="C234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="D234" s="9" t="s">
+      <c r="D234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="E234" s="9" t="s">
+      <c r="E234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="F234" s="9" t="s">
+      <c r="F234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="G234" s="9" t="s">
+      <c r="G234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="H234" s="9" t="s">
+      <c r="H234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="I234" s="9" t="s">
+      <c r="I234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="J234" s="9" t="s">
+      <c r="J234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="K234" s="9" t="s">
+      <c r="K234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="L234" s="9" t="s">
+      <c r="L234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="M234" s="9" t="s">
+      <c r="M234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="N234" s="9" t="s">
+      <c r="N234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="O234" s="9" t="s">
+      <c r="O234" s="8" t="s">
         <v>3192</v>
       </c>
-      <c r="P234" s="9" t="s">
+      <c r="P234" s="8" t="s">
         <v>3192</v>
       </c>
     </row>
@@ -26978,49 +26977,49 @@
       <c r="A235" s="1" t="s">
         <v>3193</v>
       </c>
-      <c r="B235" s="9" t="s">
+      <c r="B235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="C235" s="9" t="s">
+      <c r="C235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="D235" s="9" t="s">
+      <c r="D235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="E235" s="9" t="s">
+      <c r="E235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="F235" s="9" t="s">
+      <c r="F235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="G235" s="9" t="s">
+      <c r="G235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="H235" s="9" t="s">
+      <c r="H235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="I235" s="9" t="s">
+      <c r="I235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="J235" s="9" t="s">
+      <c r="J235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="K235" s="9" t="s">
+      <c r="K235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="L235" s="9" t="s">
+      <c r="L235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="M235" s="9" t="s">
+      <c r="M235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="N235" s="9" t="s">
+      <c r="N235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="O235" s="9" t="s">
+      <c r="O235" s="8" t="s">
         <v>3194</v>
       </c>
-      <c r="P235" s="9" t="s">
+      <c r="P235" s="8" t="s">
         <v>3194</v>
       </c>
     </row>
@@ -27028,49 +27027,49 @@
       <c r="A236" s="1" t="s">
         <v>3195</v>
       </c>
-      <c r="B236" s="9" t="s">
+      <c r="B236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="C236" s="9" t="s">
+      <c r="C236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="D236" s="9" t="s">
+      <c r="D236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="E236" s="9" t="s">
+      <c r="E236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="F236" s="9" t="s">
+      <c r="F236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="G236" s="9" t="s">
+      <c r="G236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="H236" s="9" t="s">
+      <c r="H236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="I236" s="9" t="s">
+      <c r="I236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="J236" s="9" t="s">
+      <c r="J236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="K236" s="9" t="s">
+      <c r="K236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="L236" s="9" t="s">
+      <c r="L236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="M236" s="9" t="s">
+      <c r="M236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="N236" s="9" t="s">
+      <c r="N236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="O236" s="9" t="s">
+      <c r="O236" s="8" t="s">
         <v>3196</v>
       </c>
-      <c r="P236" s="9" t="s">
+      <c r="P236" s="8" t="s">
         <v>3196</v>
       </c>
     </row>
@@ -34191,7 +34190,7 @@
       <c r="A391" s="1" t="s">
         <v>4776</v>
       </c>
-      <c r="B391" s="1" t="s">
+      <c r="B391" s="9" t="s">
         <v>4777</v>
       </c>
       <c r="C391" s="1" t="s">

</xml_diff>